<commit_message>
finished first page of spreadsheet
</commit_message>
<xml_diff>
--- a/election_predictor/minwages.xlsx
+++ b/election_predictor/minwages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="fed" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="127">
   <si>
     <t>Federal (FLSA)</t>
   </si>
@@ -456,7 +456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -484,13 +484,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="40" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -504,6 +513,10 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -517,6 +530,10 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -848,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1066,35 +1083,35 @@
       <c r="P3" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>2</v>
+      <c r="Q3" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R3" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T3">
+        <v>5.85</v>
+      </c>
+      <c r="U3">
+        <v>6.55</v>
+      </c>
+      <c r="V3">
+        <v>7.25</v>
+      </c>
+      <c r="W3" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X3" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -1226,11 +1243,11 @@
       <c r="P5" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" t="s">
-        <v>2</v>
+      <c r="Q5" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R5" s="2">
+        <v>5.15</v>
       </c>
       <c r="S5">
         <v>6.75</v>
@@ -1306,35 +1323,35 @@
       <c r="P6" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q6" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" t="s">
-        <v>71</v>
-      </c>
-      <c r="S6" t="s">
-        <v>86</v>
-      </c>
-      <c r="T6" t="s">
-        <v>87</v>
-      </c>
-      <c r="U6" t="s">
-        <v>87</v>
-      </c>
-      <c r="V6" t="s">
-        <v>86</v>
-      </c>
-      <c r="W6" t="s">
-        <v>86</v>
-      </c>
-      <c r="X6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>86</v>
+      <c r="Q6" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R6" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S6">
+        <v>6.25</v>
+      </c>
+      <c r="T6">
+        <v>6.25</v>
+      </c>
+      <c r="U6">
+        <v>6.25</v>
+      </c>
+      <c r="V6">
+        <v>6.25</v>
+      </c>
+      <c r="W6">
+        <v>6.25</v>
+      </c>
+      <c r="X6">
+        <v>6.25</v>
+      </c>
+      <c r="Y6">
+        <v>6.25</v>
+      </c>
+      <c r="Z6">
+        <v>6.25</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1706,8 +1723,8 @@
       <c r="P11" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q11" t="s">
-        <v>2</v>
+      <c r="Q11" s="2">
+        <v>5.15</v>
       </c>
       <c r="R11">
         <v>6.4</v>
@@ -1786,35 +1803,35 @@
       <c r="P12" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q12" t="s">
-        <v>72</v>
-      </c>
-      <c r="R12" t="s">
-        <v>72</v>
-      </c>
-      <c r="S12" t="s">
-        <v>72</v>
-      </c>
-      <c r="T12" t="s">
-        <v>72</v>
-      </c>
-      <c r="U12" t="s">
-        <v>72</v>
-      </c>
-      <c r="V12" t="s">
-        <v>72</v>
-      </c>
-      <c r="W12" t="s">
-        <v>72</v>
-      </c>
-      <c r="X12" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>72</v>
+      <c r="Q12" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R12" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S12">
+        <v>5.15</v>
+      </c>
+      <c r="T12">
+        <v>5.15</v>
+      </c>
+      <c r="U12">
+        <v>5.15</v>
+      </c>
+      <c r="V12">
+        <v>5.15</v>
+      </c>
+      <c r="W12">
+        <v>5.15</v>
+      </c>
+      <c r="X12">
+        <v>5.15</v>
+      </c>
+      <c r="Y12">
+        <v>5.15</v>
+      </c>
+      <c r="Z12">
+        <v>5.15</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -2026,35 +2043,35 @@
       <c r="P15">
         <v>5.5</v>
       </c>
-      <c r="Q15" t="s">
-        <v>74</v>
-      </c>
-      <c r="R15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S15" t="s">
-        <v>74</v>
-      </c>
-      <c r="T15" t="s">
-        <v>88</v>
-      </c>
-      <c r="U15" t="s">
-        <v>89</v>
-      </c>
-      <c r="V15" t="s">
-        <v>90</v>
-      </c>
-      <c r="W15" t="s">
-        <v>91</v>
-      </c>
-      <c r="X15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>91</v>
+      <c r="Q15">
+        <v>6.5</v>
+      </c>
+      <c r="R15">
+        <v>6.5</v>
+      </c>
+      <c r="S15">
+        <v>6.5</v>
+      </c>
+      <c r="T15">
+        <v>7.5</v>
+      </c>
+      <c r="U15">
+        <v>7.75</v>
+      </c>
+      <c r="V15">
+        <v>8</v>
+      </c>
+      <c r="W15">
+        <v>8.25</v>
+      </c>
+      <c r="X15">
+        <v>8.25</v>
+      </c>
+      <c r="Y15">
+        <v>8.25</v>
+      </c>
+      <c r="Z15">
+        <v>8.25</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -2106,35 +2123,35 @@
       <c r="P16" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q16" t="s">
-        <v>29</v>
-      </c>
-      <c r="R16" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" t="s">
-        <v>29</v>
-      </c>
-      <c r="T16" t="s">
-        <v>92</v>
-      </c>
-      <c r="U16" t="s">
-        <v>93</v>
-      </c>
-      <c r="V16" t="s">
-        <v>94</v>
-      </c>
-      <c r="W16" t="s">
-        <v>94</v>
-      </c>
-      <c r="X16" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>94</v>
+      <c r="Q16" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R16" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S16" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T16" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U16" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V16" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="W16">
+        <v>7.25</v>
+      </c>
+      <c r="X16">
+        <v>7.25</v>
+      </c>
+      <c r="Y16">
+        <v>7.25</v>
+      </c>
+      <c r="Z16">
+        <v>7.25</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -2426,35 +2443,35 @@
       <c r="P20" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q20" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" t="s">
-        <v>2</v>
-      </c>
-      <c r="S20" t="s">
-        <v>2</v>
-      </c>
-      <c r="T20" t="s">
-        <v>2</v>
-      </c>
-      <c r="U20" t="s">
-        <v>2</v>
-      </c>
-      <c r="V20" t="s">
-        <v>2</v>
-      </c>
-      <c r="W20" t="s">
-        <v>2</v>
-      </c>
-      <c r="X20" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>2</v>
+      <c r="Q20" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R20" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S20" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T20" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U20" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V20" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="W20" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X20" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -2746,35 +2763,35 @@
       <c r="P24" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q24" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" t="s">
-        <v>29</v>
-      </c>
-      <c r="S24" t="s">
-        <v>95</v>
-      </c>
-      <c r="T24" t="s">
-        <v>96</v>
-      </c>
-      <c r="U24" t="s">
-        <v>97</v>
-      </c>
-      <c r="V24" t="s">
-        <v>97</v>
-      </c>
-      <c r="W24" t="s">
-        <v>97</v>
-      </c>
-      <c r="X24" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>119</v>
+      <c r="Q24" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R24" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S24">
+        <v>6.95</v>
+      </c>
+      <c r="T24">
+        <v>7.15</v>
+      </c>
+      <c r="U24">
+        <v>7.4</v>
+      </c>
+      <c r="V24">
+        <v>7.4</v>
+      </c>
+      <c r="W24">
+        <v>7.4</v>
+      </c>
+      <c r="X24">
+        <v>7.4</v>
+      </c>
+      <c r="Y24">
+        <v>7.4</v>
+      </c>
+      <c r="Z24">
+        <v>8.15</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -2826,35 +2843,35 @@
       <c r="P25">
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q25" t="s">
-        <v>75</v>
-      </c>
-      <c r="R25" t="s">
-        <v>76</v>
-      </c>
-      <c r="S25" t="s">
-        <v>98</v>
-      </c>
-      <c r="T25" t="s">
-        <v>98</v>
-      </c>
-      <c r="U25" t="s">
-        <v>98</v>
-      </c>
-      <c r="V25" t="s">
-        <v>98</v>
-      </c>
-      <c r="W25" t="s">
-        <v>98</v>
-      </c>
-      <c r="X25" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>122</v>
+      <c r="Q25">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R25">
+        <v>5.25</v>
+      </c>
+      <c r="S25">
+        <v>5.25</v>
+      </c>
+      <c r="T25">
+        <v>5.25</v>
+      </c>
+      <c r="U25">
+        <v>5.25</v>
+      </c>
+      <c r="V25">
+        <v>5.25</v>
+      </c>
+      <c r="W25">
+        <v>5.25</v>
+      </c>
+      <c r="X25">
+        <v>5.25</v>
+      </c>
+      <c r="Y25">
+        <v>5.25</v>
+      </c>
+      <c r="Z25">
+        <v>6.5</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -2906,35 +2923,35 @@
       <c r="P26" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q26" t="s">
-        <v>2</v>
-      </c>
-      <c r="R26" t="s">
-        <v>2</v>
-      </c>
-      <c r="S26" t="s">
-        <v>2</v>
-      </c>
-      <c r="T26" t="s">
-        <v>2</v>
-      </c>
-      <c r="U26" t="s">
-        <v>2</v>
-      </c>
-      <c r="V26" t="s">
-        <v>2</v>
-      </c>
-      <c r="W26" t="s">
-        <v>2</v>
-      </c>
-      <c r="X26" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>2</v>
+      <c r="Q26" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R26" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S26" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T26" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U26" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V26" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="W26" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X26" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -3066,35 +3083,35 @@
       <c r="P28">
         <v>4</v>
       </c>
-      <c r="Q28" t="s">
-        <v>77</v>
-      </c>
-      <c r="R28" t="s">
-        <v>78</v>
-      </c>
-      <c r="S28" t="s">
-        <v>99</v>
-      </c>
-      <c r="T28" t="s">
-        <v>100</v>
-      </c>
-      <c r="U28" t="s">
-        <v>101</v>
-      </c>
-      <c r="V28" t="s">
-        <v>102</v>
-      </c>
-      <c r="W28" t="s">
-        <v>103</v>
-      </c>
-      <c r="X28" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>123</v>
+      <c r="Q28">
+        <v>4</v>
+      </c>
+      <c r="R28">
+        <v>4</v>
+      </c>
+      <c r="S28">
+        <v>4</v>
+      </c>
+      <c r="T28">
+        <v>4</v>
+      </c>
+      <c r="U28">
+        <v>4</v>
+      </c>
+      <c r="V28">
+        <v>4</v>
+      </c>
+      <c r="W28">
+        <v>4</v>
+      </c>
+      <c r="X28">
+        <v>4</v>
+      </c>
+      <c r="Y28">
+        <v>4</v>
+      </c>
+      <c r="Z28">
+        <v>7.9</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -3146,35 +3163,35 @@
       <c r="P29" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q29" t="s">
-        <v>64</v>
-      </c>
-      <c r="R29" t="s">
-        <v>64</v>
-      </c>
-      <c r="S29" t="s">
-        <v>64</v>
-      </c>
-      <c r="T29" t="s">
-        <v>106</v>
-      </c>
-      <c r="U29" t="s">
-        <v>107</v>
-      </c>
-      <c r="V29" t="s">
-        <v>108</v>
-      </c>
-      <c r="W29" t="s">
-        <v>108</v>
-      </c>
-      <c r="X29" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>108</v>
+      <c r="Q29" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R29" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S29" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T29" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U29" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V29">
+        <v>7.25</v>
+      </c>
+      <c r="W29" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X29" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -3238,23 +3255,23 @@
       <c r="T30">
         <v>6.33</v>
       </c>
-      <c r="U30" t="s">
-        <v>109</v>
-      </c>
-      <c r="V30" t="s">
-        <v>110</v>
-      </c>
-      <c r="W30" t="s">
-        <v>111</v>
-      </c>
-      <c r="X30" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>111</v>
+      <c r="U30" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V30" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="W30" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X30" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -3786,11 +3803,11 @@
       <c r="P37">
         <v>2.8</v>
       </c>
-      <c r="Q37" t="s">
-        <v>79</v>
-      </c>
-      <c r="R37" t="s">
-        <v>79</v>
+      <c r="Q37">
+        <v>2.8</v>
+      </c>
+      <c r="R37">
+        <v>2.8</v>
       </c>
       <c r="S37">
         <v>6.85</v>
@@ -3813,8 +3830,8 @@
       <c r="Y37">
         <v>7.85</v>
       </c>
-      <c r="Z37" t="s">
-        <v>124</v>
+      <c r="Z37">
+        <v>7.25</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -3866,35 +3883,35 @@
       <c r="P38">
         <v>2</v>
       </c>
-      <c r="Q38" t="s">
-        <v>80</v>
-      </c>
-      <c r="R38" t="s">
-        <v>81</v>
-      </c>
-      <c r="S38" t="s">
-        <v>112</v>
-      </c>
-      <c r="T38" t="s">
-        <v>113</v>
-      </c>
-      <c r="U38" t="s">
-        <v>114</v>
-      </c>
-      <c r="V38" t="s">
-        <v>115</v>
-      </c>
-      <c r="W38" t="s">
-        <v>115</v>
-      </c>
-      <c r="X38" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>115</v>
+      <c r="Q38">
+        <v>2</v>
+      </c>
+      <c r="R38">
+        <v>2</v>
+      </c>
+      <c r="S38">
+        <v>2</v>
+      </c>
+      <c r="T38">
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <v>2</v>
+      </c>
+      <c r="V38">
+        <v>2</v>
+      </c>
+      <c r="W38">
+        <v>2</v>
+      </c>
+      <c r="X38">
+        <v>2</v>
+      </c>
+      <c r="Y38">
+        <v>2</v>
+      </c>
+      <c r="Z38">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -4186,35 +4203,35 @@
       <c r="P42" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q42" t="s">
-        <v>2</v>
-      </c>
-      <c r="R42" t="s">
-        <v>2</v>
-      </c>
-      <c r="S42" t="s">
-        <v>2</v>
-      </c>
-      <c r="T42" t="s">
-        <v>2</v>
-      </c>
-      <c r="U42" t="s">
-        <v>2</v>
-      </c>
-      <c r="V42" t="s">
-        <v>2</v>
-      </c>
-      <c r="W42" t="s">
-        <v>2</v>
-      </c>
-      <c r="X42" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>2</v>
+      <c r="Q42" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R42" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S42" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T42" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U42" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V42" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="W42" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X42" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y42" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="43" spans="1:26">
@@ -4346,35 +4363,35 @@
       <c r="P44" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q44" t="s">
-        <v>2</v>
-      </c>
-      <c r="R44" t="s">
-        <v>2</v>
-      </c>
-      <c r="S44" t="s">
-        <v>2</v>
-      </c>
-      <c r="T44" t="s">
-        <v>2</v>
-      </c>
-      <c r="U44" t="s">
-        <v>2</v>
-      </c>
-      <c r="V44" t="s">
-        <v>2</v>
-      </c>
-      <c r="W44" t="s">
-        <v>2</v>
-      </c>
-      <c r="X44" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>2</v>
+      <c r="Q44" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R44" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S44" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="T44" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U44" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V44" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="W44" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X44" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="45" spans="1:26">
@@ -4586,35 +4603,35 @@
       <c r="P47">
         <v>6.75</v>
       </c>
-      <c r="Q47" t="s">
-        <v>85</v>
+      <c r="Q47">
+        <v>7</v>
       </c>
       <c r="R47">
         <v>7.25</v>
       </c>
-      <c r="S47" t="s">
-        <v>116</v>
-      </c>
-      <c r="T47" t="s">
-        <v>117</v>
-      </c>
-      <c r="U47" t="s">
-        <v>118</v>
-      </c>
-      <c r="V47" t="s">
-        <v>118</v>
-      </c>
-      <c r="W47" t="s">
-        <v>119</v>
-      </c>
-      <c r="X47" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>125</v>
+      <c r="S47">
+        <v>7.53</v>
+      </c>
+      <c r="T47">
+        <v>7.68</v>
+      </c>
+      <c r="U47">
+        <v>8.06</v>
+      </c>
+      <c r="V47">
+        <v>8.06</v>
+      </c>
+      <c r="W47">
+        <v>8.15</v>
+      </c>
+      <c r="X47">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="Y47">
+        <v>8.6</v>
+      </c>
+      <c r="Z47">
+        <v>8.73</v>
       </c>
     </row>
     <row r="48" spans="1:26">
@@ -4666,35 +4683,35 @@
       <c r="P48" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q48" t="s">
-        <v>64</v>
-      </c>
-      <c r="R48" t="s">
-        <v>64</v>
-      </c>
-      <c r="S48" t="s">
-        <v>64</v>
-      </c>
-      <c r="T48" t="s">
-        <v>106</v>
-      </c>
-      <c r="U48" t="s">
-        <v>107</v>
-      </c>
-      <c r="V48" t="s">
-        <v>108</v>
-      </c>
-      <c r="W48" t="s">
-        <v>108</v>
-      </c>
-      <c r="X48" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>108</v>
+      <c r="Q48" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R48" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="S48">
+        <v>5.15</v>
+      </c>
+      <c r="T48" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="U48" s="3">
+        <v>6.55</v>
+      </c>
+      <c r="V48" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="W48" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="X48" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Y48" s="3">
+        <v>7.25</v>
+      </c>
+      <c r="Z48" s="3">
+        <v>7.25</v>
       </c>
     </row>
     <row r="49" spans="1:26">
@@ -4826,11 +4843,11 @@
       <c r="P50" s="2">
         <v>5.15</v>
       </c>
-      <c r="Q50" t="s">
-        <v>72</v>
-      </c>
-      <c r="R50" t="s">
-        <v>72</v>
+      <c r="Q50" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="R50" s="2">
+        <v>5.15</v>
       </c>
       <c r="S50">
         <v>5.85</v>

</xml_diff>

<commit_message>
made min wage data structure
</commit_message>
<xml_diff>
--- a/election_predictor/minwages.xlsx
+++ b/election_predictor/minwages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11620" yWindow="0" windowWidth="13640" windowHeight="14620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11620" yWindow="0" windowWidth="13640" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="fed" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4662,8 +4662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="U59" sqref="U59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>